<commit_message>
added apportionment, states reprocessing
</commit_message>
<xml_diff>
--- a/output/2010-table31.xlsx
+++ b/output/2010-table31.xlsx
@@ -1569,16 +1569,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="6">
-        <v>0.003987506719561238</v>
+        <v>0.09255869550917829</v>
       </c>
       <c r="C7" s="6">
-        <v>0.002140036041477035</v>
+        <v>0.07569922773292695</v>
       </c>
       <c r="D7" s="6">
-        <v>0.002086036503427512</v>
+        <v>0.08300328292707819</v>
       </c>
       <c r="E7" s="6">
-        <v>0.001554626023581289</v>
+        <v>0.04509469448561292</v>
       </c>
     </row>
     <row r="8" ht="17" customHeight="1">

</xml_diff>